<commit_message>
template import chi nhanhs
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/ChiNhanh_ImportTemplate.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/ChiNhanh_ImportTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Số điện thoại</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Ngày hết hạn</t>
+  </si>
+  <si>
+    <t>Mã số thuế</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G2"/>
+  <dimension ref="B1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G1:G1048576"/>
+      <selection activeCell="E2" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,12 +426,13 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -437,8 +441,9 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -449,18 +454,21 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>